<commit_message>
Minor update to backend and updated vue for frontend
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\work\workspace\MBR_Live_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D17AE6A-6778-47BB-B42C-862AD446FACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C2E3FE-0B5F-4A4F-B0C4-5FA800588449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF29E016-4629-44C4-98A3-E5134BFCA941}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF29E016-4629-44C4-98A3-E5134BFCA941}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>